<commit_message>
Added RS485 modules in BOM
</commit_message>
<xml_diff>
--- a/BOM/Final.xlsx
+++ b/BOM/Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popof\Desktop\School\Summer 2018\Winery\Github\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D638ED6-1EFC-4FCD-B121-8C0414122E31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A08ABD-21C9-46A6-BF63-CCF356ACF91C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="14856" windowHeight="7080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -430,6 +430,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/products/en/rf-if-and-rfid/rf-accessories/866?k=rp-sma%20to%20ufl</t>
+  </si>
+  <si>
+    <t>RS485 to TTL</t>
+  </si>
+  <si>
+    <t>RS485 shifter for Redox</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B01FDD52Y2/ref=ppx_yo_dt_b_asin_title_o07_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>USB to RS485</t>
+  </si>
+  <si>
+    <t>Useful to read Redox data from computer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00NKAJGZM/ref=ppx_yo_dt_b_asin_title_o09_s00?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -831,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,9 +864,10 @@
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -868,7 +887,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -877,7 +896,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -901,7 +920,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -925,7 +944,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -942,14 +961,14 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F60" si="1">D5*E5</f>
+        <f t="shared" ref="F5:F62" si="1">D5*E5</f>
         <v>7.5</v>
       </c>
       <c r="G5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -973,7 +992,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -997,7 +1016,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -1015,7 +1034,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -1039,7 +1058,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1063,7 +1082,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1084,7 +1103,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1124,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -1129,7 +1148,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -1147,7 +1166,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1171,131 +1190,128 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F16" s="2"/>
-      <c r="H16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="3">
+        <v>6.99</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <f>D16*E16</f>
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="3">
+        <v>7.19</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <f>D17*E17</f>
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+      <c r="H18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="H17" s="2">
+      <c r="F19" s="2"/>
+      <c r="H19" s="2">
         <f>SUM(F:F)</f>
-        <v>1012.02</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+        <v>1026.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D20" s="3">
         <v>0.98</v>
       </c>
-      <c r="E18">
+      <c r="E20">
         <v>4</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>3.92</v>
       </c>
-      <c r="G18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D21" s="2">
         <v>2.06</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="1"/>
-        <v>4.12</v>
-      </c>
-      <c r="G19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="1"/>
-        <v>3.9000000000000004</v>
-      </c>
-      <c r="G20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.52</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="1"/>
-        <v>1.04</v>
+        <v>4.12</v>
       </c>
       <c r="G21" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
-        <v>0.45</v>
+        <v>0.65</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="1"/>
-        <v>1.8</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="G22" t="s">
         <v>73</v>
@@ -1303,65 +1319,65 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D23" s="2">
-        <v>0.65</v>
+        <v>0.52</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="1"/>
+        <v>1.04</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="1"/>
         <v>1.3</v>
-      </c>
-      <c r="G23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="1"/>
-        <v>0.94</v>
-      </c>
-      <c r="G24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="9">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>73</v>
@@ -1369,299 +1385,299 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.94</v>
+      </c>
+      <c r="G26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>98</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D28" s="9">
         <v>0.6</v>
       </c>
-      <c r="E26">
+      <c r="E28">
         <v>6</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F28" s="2">
         <f t="shared" si="1"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="G26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+      <c r="G28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>100</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D29" s="9">
         <v>0.48</v>
       </c>
-      <c r="E27">
+      <c r="E29">
         <v>6</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F29" s="2">
         <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
-      <c r="G27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>120</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>121</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D30" s="9">
         <v>1.5</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>2</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F30" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="G30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="2">
-        <v>100</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2">
-        <f>D31*E31</f>
-        <v>100</v>
-      </c>
-      <c r="G31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="9">
-        <v>3.95</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" ref="F32:F33" si="3">D32*E32</f>
-        <v>3.95</v>
-      </c>
-      <c r="G32" t="s">
-        <v>73</v>
-      </c>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="2">
+        <v>100</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <f>D33*E33</f>
+        <v>100</v>
+      </c>
+      <c r="G33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="9">
+        <v>3.95</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" ref="F34:F35" si="3">D34*E34</f>
+        <v>3.95</v>
+      </c>
+      <c r="G34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>126</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>127</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D35" s="9">
         <v>1.5</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="G33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1.19</v>
-      </c>
-      <c r="E34">
-        <v>4</v>
-      </c>
-      <c r="F34" s="2">
-        <f>D34*E34</f>
-        <v>4.76</v>
-      </c>
-      <c r="G34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" s="9">
-        <v>44.53</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" ref="F35:F37" si="4">D35*E35</f>
-        <v>44.53</v>
+      <c r="G35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.19</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" s="2">
+        <f>D36*E36</f>
+        <v>4.76</v>
+      </c>
+      <c r="G36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="9">
+        <v>44.53</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" ref="F37:F39" si="4">D37*E37</f>
+        <v>44.53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>114</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>115</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D38" s="9">
         <v>13.37</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2">
         <f t="shared" si="4"/>
         <v>13.37</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>117</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>118</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D39" s="9">
         <v>7.71</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2">
         <f t="shared" si="4"/>
         <v>7.71</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38" s="2">
-        <f t="shared" si="1"/>
-        <v>1.02</v>
-      </c>
-      <c r="G38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0.54</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-      <c r="F39" s="2">
-        <f t="shared" si="1"/>
-        <v>1.08</v>
-      </c>
-      <c r="G39" t="s">
-        <v>73</v>
-      </c>
-    </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D40" s="3">
-        <v>1.5</v>
+        <v>0.51</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1.02</v>
       </c>
       <c r="G40" t="s">
         <v>73</v>
@@ -1669,23 +1685,20 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
       </c>
       <c r="D41" s="3">
-        <v>5.0999999999999996</v>
+        <v>0.54</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" s="2">
-        <f>D41*E41</f>
-        <v>5.0999999999999996</v>
+        <f t="shared" si="1"/>
+        <v>1.08</v>
       </c>
       <c r="G41" t="s">
         <v>73</v>
@@ -1693,81 +1706,87 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>60</v>
       </c>
       <c r="D42" s="3">
-        <v>5.43</v>
+        <v>1.5</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="2">
-        <f>D42*E42</f>
-        <v>5.43</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="G42" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C43" s="4"/>
-      <c r="D43" s="3"/>
-      <c r="F43" s="2"/>
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2">
+        <f>D43*E43</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G43" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" t="s">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="D44" s="3">
-        <v>5.62</v>
+        <v>5.43</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="1"/>
-        <v>5.62</v>
+        <f>D44*E44</f>
+        <v>5.43</v>
       </c>
       <c r="G44" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="3">
-        <v>5.62</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2">
-        <f t="shared" si="1"/>
-        <v>5.62</v>
-      </c>
-      <c r="G45" t="s">
-        <v>73</v>
-      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="3"/>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D46" s="3">
         <v>5.62</v>
@@ -1785,23 +1804,20 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
       </c>
       <c r="D47" s="3">
-        <v>8.57</v>
+        <v>5.62</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" s="2">
         <f t="shared" si="1"/>
-        <v>17.14</v>
+        <v>5.62</v>
       </c>
       <c r="G47" t="s">
         <v>73</v>
@@ -1809,126 +1825,119 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
       </c>
       <c r="D48" s="3">
-        <v>7.5</v>
+        <v>5.62</v>
       </c>
       <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" si="1"/>
+        <v>5.62</v>
+      </c>
+      <c r="G48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="3">
+        <v>8.57</v>
+      </c>
+      <c r="E49">
         <v>2</v>
       </c>
-      <c r="F48" s="2">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="G48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F49" s="2"/>
+      <c r="F49" s="2">
+        <f t="shared" si="1"/>
+        <v>17.14</v>
+      </c>
+      <c r="G49" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>67</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>68</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>69</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D52" s="3">
         <v>5.63</v>
       </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2">
         <f t="shared" si="1"/>
         <v>5.63</v>
       </c>
-      <c r="G50" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="G52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>70</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>71</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D53" s="3">
         <v>21.65</v>
       </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2">
         <f t="shared" si="1"/>
         <v>21.65</v>
-      </c>
-      <c r="G51" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" t="s">
-        <v>104</v>
-      </c>
-      <c r="D52" s="9">
-        <v>13</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="G52" t="s">
-        <v>73</v>
-      </c>
-      <c r="H52" s="2">
-        <f>SUM(F:F)</f>
-        <v>1012.02</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B53" t="s">
-        <v>106</v>
-      </c>
-      <c r="C53" t="s">
-        <v>107</v>
-      </c>
-      <c r="D53" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="E53">
-        <v>2</v>
-      </c>
-      <c r="F53" s="2">
-        <f t="shared" si="1"/>
-        <v>15</v>
       </c>
       <c r="G53" t="s">
         <v>73</v>
@@ -1936,38 +1945,78 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="9">
+        <v>13</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G54" t="s">
+        <v>73</v>
+      </c>
+      <c r="H54" s="2">
+        <f>SUM(F:F)</f>
+        <v>1026.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>109</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>110</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D56" s="9">
         <v>7</v>
       </c>
-      <c r="E54">
+      <c r="E56">
         <v>2</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F56" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="G54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F55" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F56" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G56" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -1995,10 +2044,16 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F61" s="2"/>
+      <c r="F61" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F62" s="2"/>
+      <c r="F62" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F63" s="2"/>
@@ -2195,15 +2250,23 @@
     <row r="127" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F127" s="2"/>
     </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F128" s="2"/>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F129" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C48" r:id="rId1" xr:uid="{D3E478ED-7BA4-475A-BFDB-72018A23FE81}"/>
-    <hyperlink ref="C47" r:id="rId2" xr:uid="{42D5E3C6-58CB-416C-9C34-59249A91B815}"/>
+    <hyperlink ref="C50" r:id="rId1" xr:uid="{D3E478ED-7BA4-475A-BFDB-72018A23FE81}"/>
+    <hyperlink ref="C49" r:id="rId2" xr:uid="{42D5E3C6-58CB-416C-9C34-59249A91B815}"/>
     <hyperlink ref="C7" r:id="rId3" xr:uid="{87B050BF-5AA3-4F93-AA52-1E9C2E2CD5C8}"/>
     <hyperlink ref="C6" r:id="rId4" xr:uid="{0AF02C15-CCBF-4F98-84AF-720221BD02DE}"/>
     <hyperlink ref="C10" r:id="rId5" xr:uid="{21712CE9-14B9-4AC2-8242-54A359ADA262}"/>
+    <hyperlink ref="C17" r:id="rId6" xr:uid="{ABC3FEF5-3DBD-4DB0-8426-89B26EF964AA}"/>
+    <hyperlink ref="C16" r:id="rId7" xr:uid="{48515240-4945-4B26-96E2-235AAA569296}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>